<commit_message>
Update code for demo - Good luck to me ^^
</commit_message>
<xml_diff>
--- a/TestData/group.xlsx
+++ b/TestData/group.xlsx
@@ -38,9 +38,6 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>Group 1 from Excel</t>
-  </si>
-  <si>
     <t>This group is created by get data from excel file</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Group 2 from Excel</t>
+  </si>
+  <si>
+    <t>Group UI Automation</t>
   </si>
 </sst>
 </file>
@@ -368,13 +368,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -394,21 +394,21 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>